<commit_message>
Add output_consolidated_trial_balance folder, output package, and FolderOutput class. Clean up code by eliminating console prints for testing other classes.
</commit_message>
<xml_diff>
--- a/src/Trial_Balance_Template.xlsx
+++ b/src/Trial_Balance_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Dev/Personal/Consolidation_Tool_Java/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{670B1E45-6ED7-B743-AD8D-DE6D78D11207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1848CBF5-1621-2840-905F-62303ABC5286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27160" windowHeight="16440" xr2:uid="{F427E4EB-3158-E540-BE3D-447F6EFEC94C}"/>
+    <workbookView xWindow="740" yWindow="1000" windowWidth="27160" windowHeight="16440" xr2:uid="{F427E4EB-3158-E540-BE3D-447F6EFEC94C}"/>
   </bookViews>
   <sheets>
     <sheet name="Trial_Balance" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>